<commit_message>
Added gitignores, updated experiment list
</commit_message>
<xml_diff>
--- a/Code/Tractor Beam/output/Experiment List.xlsx
+++ b/Code/Tractor Beam/output/Experiment List.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\Projects\Omnimagnet\Code\Tractor Beam\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CAC030-F65F-4D91-9F52-948EC7BEC290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E2C8CD-0923-4DF5-816B-3E2CEE533418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiment Table" sheetId="1" r:id="rId1"/>
     <sheet name="Object List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,18 +36,204 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="18">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="18">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
   <si>
     <t>Experiment</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Setup</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -58,9 +244,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>Objects</t>
   </si>
   <si>
     <t>Aluminum Balls</t>
@@ -91,19 +274,10 @@
     <t>E</t>
   </si>
   <si>
-    <t>Large Behind Small</t>
-  </si>
-  <si>
     <t>2" Aluminum Ball
 1" Aluminum Ball?</t>
   </si>
   <si>
-    <t>Small Behind Large</t>
-  </si>
-  <si>
-    <t>2 Large Rafts Aligned, large sphere closer</t>
-  </si>
-  <si>
     <t>Copper Disks</t>
   </si>
   <si>
@@ -118,13 +292,151 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>Experiment Category</t>
+  </si>
+  <si>
+    <t>Objects Included</t>
+  </si>
+  <si>
+    <t>Raft Diameters</t>
+  </si>
+  <si>
+    <t>3x 100mm</t>
+  </si>
+  <si>
+    <t>2x 100mm</t>
+  </si>
+  <si>
+    <t>2" Aluminum Sphere
+1.25" Aluminum Sphere
+1" Aluminum Sphere</t>
+  </si>
+  <si>
+    <t>1" Aluminum Sphere
+1.25" Aluminum Sphere
+2" Aluminum Sphere</t>
+  </si>
+  <si>
+    <t>Far raft drifts away, middle raft collides into front raft and gets pulled in</t>
+  </si>
+  <si>
+    <t>Back raft collides into middle raft which then collides into front raft, rotate to get pulled in but hit wall</t>
+  </si>
+  <si>
+    <t>3 Aluminum spheres of differing sizes placed inline moving away from magnet. Ordered largest to smallest with largest closest to magnet</t>
+  </si>
+  <si>
+    <t>3 Aluminum spheres of differing sizes placed inline moving away from magnet. Ordered smallest to largest with smallest closest to magnet</t>
+  </si>
+  <si>
+    <t>2 Aluminum spheres of differing sizes placed inline moving away form magnet. Ordered with smallest closer to magnet</t>
+  </si>
+  <si>
+    <t>Back raft catches up to and collides with front raft after it passes magnet plane</t>
+  </si>
+  <si>
+    <t>(Note: Rafts spaced same as C1 but placed further away)
+Both rafts drift off to the side.</t>
+  </si>
+  <si>
+    <t>(Note: Rafts placed same as C2) Both Rafts Drift in at similar paces</t>
+  </si>
+  <si>
+    <t>Back raft rapidly catches up to smaller front raft and swings it around</t>
+  </si>
+  <si>
+    <t>2 Aluminum spheres of differing sizes placed inline moving away form magnet. Ordered with largest closer to magnet</t>
+  </si>
+  <si>
+    <t>Back raft catches up to front raft and swings around as both get pulled in</t>
+  </si>
+  <si>
+    <t>Back raft slowly gets pulled into seemingly unmoving front raft and collides (ended early due to magnet heat)</t>
+  </si>
+  <si>
+    <t>Back raft gets pulled into front raft</t>
+  </si>
+  <si>
+    <t>Back raft collides into front raft then gets knocked into wall</t>
+  </si>
+  <si>
+    <t>Back raft collides into front raft and both get pulled in.</t>
+  </si>
+  <si>
+    <t>Video 1 Image</t>
+  </si>
+  <si>
+    <t>Video 3 Image</t>
+  </si>
+  <si>
+    <t>Video 1 Description</t>
+  </si>
+  <si>
+    <t>Video 2 Description</t>
+  </si>
+  <si>
+    <t>Video 3 Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video 2 Image </t>
+  </si>
+  <si>
+    <t>Experiment Variation</t>
+  </si>
+  <si>
+    <t>Small Closer</t>
+  </si>
+  <si>
+    <t>Large Closer</t>
+  </si>
+  <si>
+    <t>Object Size</t>
+  </si>
+  <si>
+    <t>Video 4 Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video 5 Image </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video 4 Image </t>
+  </si>
+  <si>
+    <t>Detailed Description</t>
+  </si>
+  <si>
+    <t>Layout Photo</t>
+  </si>
+  <si>
+    <t>Materials Included</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Video 5 Description</t>
+  </si>
+  <si>
+    <t>Reversed Experiment</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>1" Aluminum Ball
+2" Aluminum Ball?</t>
+  </si>
+  <si>
+    <t>2 Aluminum spheres of differing sizes placed inline moving away from magnet. Ordered with largest closer to magnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,13 +444,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,25 +494,204 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="28"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -182,6 +702,183 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="18">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+</richValueRels>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFBABB81-F512-4DBE-8388-A4335625DAAC}" name="ExperimentTable" displayName="ExperimentTable" ref="A1:S200" totalsRowShown="0" headerRowDxfId="13" dataDxfId="14">
+  <autoFilter ref="A1:S200" xr:uid="{EFBABB81-F512-4DBE-8388-A4335625DAAC}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{4DD7D756-79AC-47EF-9C53-25636B1735E5}" name="Experiment" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{A5508EBB-85DA-455E-A1FA-9E56CBEDB2BC}" name="Experiment Category" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{EDC4A070-C179-4879-9161-0E6CEE3B03CE}" name="Experiment Variation" dataDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{29A16266-4960-4FC1-9E77-B1F193F89510}" name="Materials Included" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{391AE230-BEFE-47D0-B901-B18AD8DA3BAD}" name="Reversed Experiment" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{07EC9780-17F5-4E52-B720-72C36789D114}" name="Objects Included" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{E3D8272A-32FA-46B4-9CED-819AE69A7AFC}" name="Layout Photo" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{03820AD5-F5CC-48D3-A203-36988C3D0FE2}" name="Detailed Description" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{4E9FB0B1-757E-473D-A861-553A2A29B87E}" name="Raft Diameters" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{332FF9F0-17E8-45B7-B0F2-B09318E62092}" name="Video 1 Image" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{94CD7315-5538-435F-83A9-A4CC877D8039}" name="Video 1 Description" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{6E20D435-E90D-4EFA-9D84-1818E4341414}" name="Video 2 Image " dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{5CFF4F8D-912F-46F5-B8B4-BD7928214C8F}" name="Video 2 Description" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{D5353BFF-361F-44D5-A6B3-B447B5753E0B}" name="Video 3 Image" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{48E41B14-A242-44C3-A9AE-9B7341E870C1}" name="Video 3 Description" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{951F86DC-1089-4B6A-8332-CFFD9F647F43}" name="Video 4 Image " dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{4D8E6062-AA59-4A22-8DF7-99FB720B878C}" name="Video 4 Description" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{C4E2EB3A-F870-4D7F-8469-AB06B6E5EBBD}" name="Video 5 Image " dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{080AA4D1-4987-4928-BBC4-0F2C293734F6}" name="Video 5 Description" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,116 +1144,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.7890625" customWidth="1"/>
-    <col min="2" max="2" width="25.7890625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.1015625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.41796875" style="5" customWidth="1"/>
+    <col min="2" max="5" width="27.41796875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="27.41796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.15625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="37.578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.05078125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5234375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.41796875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="37.5234375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.41796875" style="7" customWidth="1"/>
+    <col min="14" max="14" width="37.7890625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="27.41796875" style="7" customWidth="1"/>
+    <col min="16" max="16" width="37.83984375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="27.41796875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="37.9453125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="27.41796875" style="2" customWidth="1"/>
+    <col min="20" max="25" width="27.41796875" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="16384" width="27.41796875" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="1" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="2" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="G7" s="3" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="2" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="J8" s="1" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="1" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J1:S200">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ISBLANK(J1)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -572,62 +1559,62 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Experiment List Updates
</commit_message>
<xml_diff>
--- a/Code/Tractor Beam/output/Experiment List.xlsx
+++ b/Code/Tractor Beam/output/Experiment List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\Projects\Omnimagnet\Code\Tractor Beam\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E2C8CD-0923-4DF5-816B-3E2CEE533418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFBF2DC-9819-4DB4-91E6-4659B4B091C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="18">
+  <futureMetadata name="XLRICHVALUE" count="20">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -168,8 +168,22 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="18">
+  <valueMetadata count="20">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -223,13 +237,19 @@
     </bk>
     <bk>
       <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
   <si>
     <t>Experiment</t>
   </si>
@@ -337,13 +357,6 @@
     <t>Back raft catches up to and collides with front raft after it passes magnet plane</t>
   </si>
   <si>
-    <t>(Note: Rafts spaced same as C1 but placed further away)
-Both rafts drift off to the side.</t>
-  </si>
-  <si>
-    <t>(Note: Rafts placed same as C2) Both Rafts Drift in at similar paces</t>
-  </si>
-  <si>
     <t>Back raft rapidly catches up to smaller front raft and swings it around</t>
   </si>
   <si>
@@ -430,6 +443,48 @@
   </si>
   <si>
     <t>2 Aluminum spheres of differing sizes placed inline moving away from magnet. Ordered with largest closer to magnet</t>
+  </si>
+  <si>
+    <t>Front raft basically sits still while back raft very very slowly moves towards it</t>
+  </si>
+  <si>
+    <t>Front raft very very slowly inches forward, back raft moves forward slightly quicker but still very slow</t>
+  </si>
+  <si>
+    <t>Both rafts drift off to the side.</t>
+  </si>
+  <si>
+    <t>Both Rafts Drift in at similar paces</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Object Distance</t>
+  </si>
+  <si>
+    <t>0.25" Aluminum Ball</t>
+  </si>
+  <si>
+    <t>1" Aluminum Ball</t>
+  </si>
+  <si>
+    <t>2" Aluminum Ball</t>
+  </si>
+  <si>
+    <t>3 Rafts Inline</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>3 Aluminum spheres of the same size placed inline moving away from magnet spaced equally apart.</t>
   </si>
 </sst>
 </file>
@@ -526,6 +581,55 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -545,13 +649,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -571,70 +668,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -684,6 +717,28 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="28"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -745,7 +800,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="18">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="20">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -816,6 +871,14 @@
   </rv>
   <rv s="0">
     <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -850,32 +913,34 @@
   <rel r:id="rId16"/>
   <rel r:id="rId17"/>
   <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
 </richValueRels>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFBABB81-F512-4DBE-8388-A4335625DAAC}" name="ExperimentTable" displayName="ExperimentTable" ref="A1:S200" totalsRowShown="0" headerRowDxfId="13" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFBABB81-F512-4DBE-8388-A4335625DAAC}" name="ExperimentTable" displayName="ExperimentTable" ref="A1:S200" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:S200" xr:uid="{EFBABB81-F512-4DBE-8388-A4335625DAAC}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{4DD7D756-79AC-47EF-9C53-25636B1735E5}" name="Experiment" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{A5508EBB-85DA-455E-A1FA-9E56CBEDB2BC}" name="Experiment Category" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{EDC4A070-C179-4879-9161-0E6CEE3B03CE}" name="Experiment Variation" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{29A16266-4960-4FC1-9E77-B1F193F89510}" name="Materials Included" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{391AE230-BEFE-47D0-B901-B18AD8DA3BAD}" name="Reversed Experiment" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{07EC9780-17F5-4E52-B720-72C36789D114}" name="Objects Included" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{E3D8272A-32FA-46B4-9CED-819AE69A7AFC}" name="Layout Photo" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{03820AD5-F5CC-48D3-A203-36988C3D0FE2}" name="Detailed Description" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{4DD7D756-79AC-47EF-9C53-25636B1735E5}" name="Experiment" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{A5508EBB-85DA-455E-A1FA-9E56CBEDB2BC}" name="Experiment Category" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{EDC4A070-C179-4879-9161-0E6CEE3B03CE}" name="Experiment Variation" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{29A16266-4960-4FC1-9E77-B1F193F89510}" name="Materials Included" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{391AE230-BEFE-47D0-B901-B18AD8DA3BAD}" name="Reversed Experiment" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{07EC9780-17F5-4E52-B720-72C36789D114}" name="Objects Included" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E3D8272A-32FA-46B4-9CED-819AE69A7AFC}" name="Layout Photo" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{03820AD5-F5CC-48D3-A203-36988C3D0FE2}" name="Detailed Description" dataDxfId="12"/>
     <tableColumn id="7" xr3:uid="{4E9FB0B1-757E-473D-A861-553A2A29B87E}" name="Raft Diameters" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{332FF9F0-17E8-45B7-B0F2-B09318E62092}" name="Video 1 Image" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{94CD7315-5538-435F-83A9-A4CC877D8039}" name="Video 1 Description" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{6E20D435-E90D-4EFA-9D84-1818E4341414}" name="Video 2 Image " dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{5CFF4F8D-912F-46F5-B8B4-BD7928214C8F}" name="Video 2 Description" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{D5353BFF-361F-44D5-A6B3-B447B5753E0B}" name="Video 3 Image" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{48E41B14-A242-44C3-A9AE-9B7341E870C1}" name="Video 3 Description" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{332FF9F0-17E8-45B7-B0F2-B09318E62092}" name="Video 1 Image" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{94CD7315-5538-435F-83A9-A4CC877D8039}" name="Video 1 Description" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{6E20D435-E90D-4EFA-9D84-1818E4341414}" name="Video 2 Image " dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{5CFF4F8D-912F-46F5-B8B4-BD7928214C8F}" name="Video 2 Description" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{D5353BFF-361F-44D5-A6B3-B447B5753E0B}" name="Video 3 Image" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{48E41B14-A242-44C3-A9AE-9B7341E870C1}" name="Video 3 Description" dataDxfId="5"/>
     <tableColumn id="14" xr3:uid="{951F86DC-1089-4B6A-8332-CFFD9F647F43}" name="Video 4 Image " dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{4D8E6062-AA59-4A22-8DF7-99FB720B878C}" name="Video 4 Description" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{C4E2EB3A-F870-4D7F-8469-AB06B6E5EBBD}" name="Video 5 Image " dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{080AA4D1-4987-4928-BBC4-0F2C293734F6}" name="Video 5 Description" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{4D8E6062-AA59-4A22-8DF7-99FB720B878C}" name="Video 4 Description" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{C4E2EB3A-F870-4D7F-8469-AB06B6E5EBBD}" name="Video 5 Image " dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{080AA4D1-4987-4928-BBC4-0F2C293734F6}" name="Video 5 Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1144,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1181,55 +1246,55 @@
         <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="P1" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1237,13 +1302,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>2</v>
@@ -1278,13 +1343,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>1</v>
@@ -1313,16 +1378,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1346,13 +1411,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="N4" s="2" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1360,13 +1425,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>13</v>
@@ -1387,7 +1452,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="2" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1395,13 +1472,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>4</v>
@@ -1409,26 +1486,26 @@
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3" t="e" vm="12">
+      <c r="G6" s="3" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="1" t="e" vm="13">
+      <c r="J6" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="1" t="e" vm="13">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1436,13 +1513,13 @@
         <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>19</v>
@@ -1450,20 +1527,20 @@
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="e" vm="14">
+      <c r="G7" s="3" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="2" t="e" vm="15">
+      <c r="N7" s="2" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1471,13 +1548,13 @@
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>17</v>
@@ -1485,7 +1562,7 @@
       <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3" t="e" vm="16">
+      <c r="G8" s="3" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1494,48 +1571,126 @@
       <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="1" t="e" vm="17">
+      <c r="J8" s="1" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="1" t="e" vm="18">
+        <v>38</v>
+      </c>
+      <c r="L8" s="1" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="10" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J1:S200">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISBLANK(J1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Generated Videos for H1, H2, H3, E3
</commit_message>
<xml_diff>
--- a/Code/Tractor Beam/output/Experiment List.xlsx
+++ b/Code/Tractor Beam/output/Experiment List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\Projects\Omnimagnet\Code\Tractor Beam\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFBF2DC-9819-4DB4-91E6-4659B4B091C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0866DA-77CE-41EF-8247-6B3E37FD5012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="20">
+  <futureMetadata name="XLRICHVALUE" count="25">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -182,8 +182,43 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="20"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="21"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="22"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="23"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="24"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="20">
+  <valueMetadata count="25">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -243,13 +278,28 @@
     </bk>
     <bk>
       <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
+    </bk>
+    <bk>
+      <rc t="1" v="22"/>
+    </bk>
+    <bk>
+      <rc t="1" v="23"/>
+    </bk>
+    <bk>
+      <rc t="1" v="24"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
   <si>
     <t>Experiment</t>
   </si>
@@ -432,9 +482,6 @@
     <t>Video 5 Description</t>
   </si>
   <si>
-    <t>Reversed Experiment</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -481,10 +528,34 @@
     <t>3 Rafts Inline</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>3 Aluminum spheres of the same size placed inline moving away from magnet spaced equally apart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back raft somewhat drifts away then stays stationary. Front raft very slowly drifts in </t>
+  </si>
+  <si>
+    <t>Front raft drifts backwards and back raft collides into it</t>
+  </si>
+  <si>
+    <t>Front raft gets pulled in. Back raft starts getting pulled in then drifts backwards then gets pulled in</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Experiment Group</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>IJK</t>
   </si>
 </sst>
 </file>
@@ -523,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,6 +604,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -574,6 +663,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -800,7 +898,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="20">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="25">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -879,6 +977,26 @@
   </rv>
   <rv s="0">
     <v>19</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>20</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>21</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>22</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>23</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>24</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -915,6 +1033,11 @@
   <rel r:id="rId18"/>
   <rel r:id="rId19"/>
   <rel r:id="rId20"/>
+  <rel r:id="rId21"/>
+  <rel r:id="rId22"/>
+  <rel r:id="rId23"/>
+  <rel r:id="rId24"/>
+  <rel r:id="rId25"/>
 </richValueRels>
 </file>
 
@@ -926,7 +1049,7 @@
     <tableColumn id="2" xr3:uid="{A5508EBB-85DA-455E-A1FA-9E56CBEDB2BC}" name="Experiment Category" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{EDC4A070-C179-4879-9161-0E6CEE3B03CE}" name="Experiment Variation" dataDxfId="17"/>
     <tableColumn id="18" xr3:uid="{29A16266-4960-4FC1-9E77-B1F193F89510}" name="Materials Included" dataDxfId="16"/>
-    <tableColumn id="19" xr3:uid="{391AE230-BEFE-47D0-B901-B18AD8DA3BAD}" name="Reversed Experiment" dataDxfId="15"/>
+    <tableColumn id="19" xr3:uid="{391AE230-BEFE-47D0-B901-B18AD8DA3BAD}" name="Experiment Group" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{07EC9780-17F5-4E52-B720-72C36789D114}" name="Objects Included" dataDxfId="14"/>
     <tableColumn id="5" xr3:uid="{E3D8272A-32FA-46B4-9CED-819AE69A7AFC}" name="Layout Photo" dataDxfId="13"/>
     <tableColumn id="6" xr3:uid="{03820AD5-F5CC-48D3-A203-36988C3D0FE2}" name="Detailed Description" dataDxfId="12"/>
@@ -1211,9 +1334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1252,7 +1375,7 @@
         <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>21</v>
@@ -1311,7 +1434,7 @@
         <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
@@ -1328,13 +1451,13 @@
       <c r="J2" s="1" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="1" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1352,7 +1475,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
@@ -1369,7 +1492,7 @@
       <c r="J3" s="1" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1387,7 +1510,7 @@
         <v>56</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1404,20 +1527,20 @@
       <c r="J4" s="1" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L4" s="1" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="2" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="N4" s="2" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1434,7 +1557,7 @@
         <v>56</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
@@ -1451,20 +1574,20 @@
       <c r="J5" s="1" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="9" t="s">
         <v>33</v>
       </c>
       <c r="L5" s="1" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="2" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O5" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="N5" s="2" t="e" vm="13">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1481,7 +1604,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
@@ -1498,14 +1621,20 @@
       <c r="J6" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="10" t="s">
         <v>35</v>
       </c>
       <c r="L6" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="10" t="s">
         <v>36</v>
+      </c>
+      <c r="N6" s="2" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1522,12 +1651,12 @@
         <v>56</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="e" vm="16">
+      <c r="G7" s="3" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -1536,10 +1665,10 @@
       <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="2" t="e" vm="17">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O7" s="7" t="s">
+      <c r="N7" s="2" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O7" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1557,12 +1686,12 @@
         <v>56</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3" t="e" vm="18">
+      <c r="G8" s="3" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1571,22 +1700,22 @@
       <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="1" t="e" vm="19">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="1" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="1" t="e" vm="20">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M8" s="7" t="s">
+      <c r="L8" s="1" t="e" vm="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>49</v>
@@ -1598,39 +1727,60 @@
         <v>56</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3" t="e" vm="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="J9" s="1" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="1" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="2" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>23</v>
@@ -1638,25 +1788,25 @@
     </row>
     <row r="11" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>23</v>
@@ -1664,25 +1814,25 @@
     </row>
     <row r="12" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="C12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Generated F1, F2, G3 videos
</commit_message>
<xml_diff>
--- a/Code/Tractor Beam/output/Experiment List.xlsx
+++ b/Code/Tractor Beam/output/Experiment List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\Projects\Omnimagnet\Code\Tractor Beam\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0866DA-77CE-41EF-8247-6B3E37FD5012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D385674-85B0-4BE6-A437-3172DBF429D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="25">
+  <futureMetadata name="XLRICHVALUE" count="28">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -217,8 +217,29 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="25"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="26"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="27"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="25">
+  <valueMetadata count="28">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -293,13 +314,22 @@
     </bk>
     <bk>
       <rc t="1" v="24"/>
+    </bk>
+    <bk>
+      <rc t="1" v="25"/>
+    </bk>
+    <bk>
+      <rc t="1" v="26"/>
+    </bk>
+    <bk>
+      <rc t="1" v="27"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>Experiment</t>
   </si>
@@ -540,22 +570,31 @@
     <t>Front raft gets pulled in. Back raft starts getting pulled in then drifts backwards then gets pulled in</t>
   </si>
   <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
     <t>Experiment Group</t>
   </si>
   <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>FG</t>
-  </si>
-  <si>
-    <t>IJK</t>
+    <t>Back raft collides into an unmoving front raft and gets pulled in slowly while pushing front raft aside</t>
+  </si>
+  <si>
+    <t>Both rafts slowly drift up and back away from magnets at start then start getting pulled back towards the magnets. Back raft with smaller object pulled faster and collides into front raft</t>
+  </si>
+  <si>
+    <t>Both rafts drift back to start then get pulled in with small raft in back being faster</t>
+  </si>
+  <si>
+    <t>A-B</t>
+  </si>
+  <si>
+    <t>C-H</t>
+  </si>
+  <si>
+    <t>D-E</t>
+  </si>
+  <si>
+    <t>F-G</t>
+  </si>
+  <si>
+    <t>I-J-K</t>
   </si>
 </sst>
 </file>
@@ -898,7 +937,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="25">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="28">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -997,6 +1036,18 @@
   </rv>
   <rv s="0">
     <v>24</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>25</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>26</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>27</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -1038,6 +1089,9 @@
   <rel r:id="rId23"/>
   <rel r:id="rId24"/>
   <rel r:id="rId25"/>
+  <rel r:id="rId26"/>
+  <rel r:id="rId27"/>
+  <rel r:id="rId28"/>
 </richValueRels>
 </file>
 
@@ -1334,15 +1388,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.41796875" style="5" customWidth="1"/>
-    <col min="2" max="5" width="27.41796875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.3125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.3125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.578125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="27.41796875" style="6" customWidth="1"/>
     <col min="6" max="6" width="27.41796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="37.15625" style="3" customWidth="1"/>
     <col min="8" max="8" width="37.578125" style="7" customWidth="1"/>
@@ -1375,7 +1433,7 @@
         <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>21</v>
@@ -1434,7 +1492,7 @@
         <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
@@ -1475,7 +1533,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
@@ -1510,7 +1568,7 @@
         <v>56</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1557,7 +1615,7 @@
         <v>56</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
@@ -1604,7 +1662,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
@@ -1651,7 +1709,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
@@ -1665,7 +1723,19 @@
       <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="2" t="e" vm="18">
+      <c r="J7" s="1" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="1" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="2" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="O7" s="10" t="s">
@@ -1686,12 +1756,12 @@
         <v>56</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3" t="e" vm="19">
+      <c r="G8" s="3" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1700,17 +1770,23 @@
       <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="1" t="e" vm="20">
+      <c r="J8" s="1" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="1" t="e" vm="21">
+      <c r="L8" s="1" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>39</v>
+      </c>
+      <c r="N8" s="2" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1727,12 +1803,12 @@
         <v>56</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="3" t="e" vm="22">
+      <c r="G9" s="3" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -1741,19 +1817,19 @@
       <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="1" t="e" vm="23">
+      <c r="J9" s="1" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="1" t="e" vm="24">
+      <c r="L9" s="1" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="2" t="e" vm="25">
+      <c r="N9" s="2" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="10" t="s">
@@ -1774,7 +1850,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>69</v>
@@ -1800,7 +1876,7 @@
         <v>56</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>70</v>
@@ -1826,7 +1902,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
New 3-piece raft alignment design
</commit_message>
<xml_diff>
--- a/Code/Tractor Beam/output/Experiment List.xlsx
+++ b/Code/Tractor Beam/output/Experiment List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\Projects\Omnimagnet\Code\Tractor Beam\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D385674-85B0-4BE6-A437-3172DBF429D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416F4502-7679-4686-B49F-B7EE9F526161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="28">
+  <futureMetadata name="XLRICHVALUE" count="31">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -238,8 +238,29 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="28"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="29"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="30"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="28">
+  <valueMetadata count="31">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -323,13 +344,22 @@
     </bk>
     <bk>
       <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="89">
   <si>
     <t>Experiment</t>
   </si>
@@ -595,6 +625,15 @@
   </si>
   <si>
     <t>I-J-K</t>
+  </si>
+  <si>
+    <t>Back raft collides into middle raft which then collides into front raft and they slowly get pulled in with some lateral movement due to contact</t>
+  </si>
+  <si>
+    <t>Back raft quickly slams into middle raft, front raft gets sucked in first while back two slowly drift in</t>
+  </si>
+  <si>
+    <t>Middle raft collides into front and both get pulled in faster than the back raft.</t>
   </si>
 </sst>
 </file>
@@ -937,7 +976,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="28">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="31">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -1048,6 +1087,18 @@
   </rv>
   <rv s="0">
     <v>27</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>28</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>29</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>30</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -1092,6 +1143,9 @@
   <rel r:id="rId26"/>
   <rel r:id="rId27"/>
   <rel r:id="rId28"/>
+  <rel r:id="rId29"/>
+  <rel r:id="rId30"/>
+  <rel r:id="rId31"/>
 </richValueRels>
 </file>
 
@@ -1389,10 +1443,10 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1518,6 +1572,12 @@
       <c r="M2" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="N2" s="2" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
@@ -1538,7 +1598,7 @@
       <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="3" t="e" vm="4">
+      <c r="G3" s="3" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="H3" s="7" t="s">
@@ -1547,11 +1607,23 @@
       <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="e" vm="5">
+      <c r="J3" s="1" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>28</v>
+      </c>
+      <c r="L3" s="1" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="2" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1573,7 +1645,7 @@
       <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="3" t="e" vm="6">
+      <c r="G4" s="3" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -1582,19 +1654,19 @@
       <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="e" vm="7">
+      <c r="J4" s="1" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="1" t="e" vm="8">
+      <c r="L4" s="1" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="2" t="e" vm="9">
+      <c r="N4" s="2" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="O4" s="11" t="s">
@@ -1620,7 +1692,7 @@
       <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="e" vm="10">
+      <c r="G5" s="3" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -1629,19 +1701,19 @@
       <c r="I5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="1" t="e" vm="11">
+      <c r="J5" s="1" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="1" t="e" vm="12">
+      <c r="L5" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="N5" s="2" t="e" vm="13">
+      <c r="N5" s="2" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="O5" s="9" t="s">
@@ -1667,7 +1739,7 @@
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3" t="e" vm="14">
+      <c r="G6" s="3" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -1676,19 +1748,19 @@
       <c r="I6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="1" t="e" vm="15">
+      <c r="J6" s="1" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="1" t="e" vm="15">
+      <c r="L6" s="1" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="2" t="e" vm="16">
+      <c r="N6" s="2" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="O6" s="11" t="s">
@@ -1714,7 +1786,7 @@
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="e" vm="17">
+      <c r="G7" s="3" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -1723,19 +1795,19 @@
       <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="1" t="e" vm="18">
+      <c r="J7" s="1" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="L7" s="1" t="e" vm="19">
+      <c r="L7" s="1" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="N7" s="2" t="e" vm="20">
+      <c r="N7" s="2" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="O7" s="10" t="s">
@@ -1761,7 +1833,7 @@
       <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3" t="e" vm="21">
+      <c r="G8" s="3" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1770,19 +1842,19 @@
       <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="1" t="e" vm="22">
+      <c r="J8" s="1" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="1" t="e" vm="23">
+      <c r="L8" s="1" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="2" t="e" vm="24">
+      <c r="N8" s="2" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
       <c r="O8" s="11" t="s">
@@ -1808,7 +1880,7 @@
       <c r="F9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="3" t="e" vm="25">
+      <c r="G9" s="3" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -1817,19 +1889,19 @@
       <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="1" t="e" vm="26">
+      <c r="J9" s="1" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="1" t="e" vm="27">
+      <c r="L9" s="1" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="2" t="e" vm="28">
+      <c r="N9" s="2" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="10" t="s">
@@ -1853,7 +1925,7 @@
         <v>85</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>73</v>
@@ -1905,7 +1977,7 @@
         <v>85</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>73</v>

</xml_diff>